<commit_message>
Korekty po uwagach Taty cz.1
</commit_message>
<xml_diff>
--- a/pomocnicze/analiza demograficzna studentów.xlsx
+++ b/pomocnicze/analiza demograficzna studentów.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPSZ\Desktop\STUDIA\doktorat_git\pomocnicze\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84CF6B9-B04E-4D3B-B3C3-8A7A97ADF341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60F6A55-A8C7-409B-99AF-972987840B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2160" yWindow="-21730" windowWidth="37730" windowHeight="21860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1830" yWindow="-21710" windowWidth="37380" windowHeight="21820" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabl.1_ogółem" sheetId="1" r:id="rId1"/>
@@ -206,12 +206,6 @@
     <t>Liczba studentów</t>
   </si>
   <si>
-    <t>Liczba osób w wieku 19-24 lata</t>
-  </si>
-  <si>
-    <t>Udział liczby studentów w liczbie osób w wieku 19-24 lata</t>
-  </si>
-  <si>
     <t>Suma z Wartosc</t>
   </si>
   <si>
@@ -352,6 +346,12 @@
   <si>
     <t>Szkoły i ich finanse 2021</t>
   </si>
+  <si>
+    <t>Udział liczby studentów w liczbie osób w wieku 19-24 lat</t>
+  </si>
+  <si>
+    <t>Liczba osób w wieku 19-24 lat</t>
+  </si>
 </sst>
 </file>
 
@@ -363,7 +363,7 @@
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0\ _z_ł_-;\-* #,##0\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -968,6 +968,12 @@
     <xf numFmtId="1" fontId="20" fillId="0" borderId="8" xfId="28" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -984,12 +990,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="20" fillId="0" borderId="1" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1113,7 +1113,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Liczba osób w wieku 19-24 lata</c:v>
+                  <c:v>Liczba osób w wieku 19-24 lat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1962,7 +1962,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lata</c:v>
+                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lat</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2453,7 +2453,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Liczba osób w wieku 19-24 lata</c:v>
+                  <c:v>Liczba osób w wieku 19-24 lat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3206,7 +3206,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lata</c:v>
+                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lat</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -4815,7 +4815,7 @@
     <c:legend>
       <c:legendPos val="b"/>
       <c:legendEntry>
-        <c:idx val="2"/>
+        <c:idx val="0"/>
         <c:delete val="1"/>
       </c:legendEntry>
       <c:layout>
@@ -4938,7 +4938,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Liczba osób w wieku 19-24 lata</c:v>
+                  <c:v>Liczba osób w wieku 19-24 lat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5758,7 +5758,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lata</c:v>
+                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lat</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -6202,7 +6202,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Liczba osób w wieku 19-24 lata</c:v>
+                  <c:v>Liczba osób w wieku 19-24 lat</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7056,7 +7056,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lata</c:v>
+                        <c:v>Udział liczby studentów w liczbie osób w wieku 19-24 lat</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -12159,13 +12159,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="2" t="s">
@@ -12278,23 +12278,23 @@
     </row>
     <row r="6" spans="1:33">
       <c r="A6" s="55"/>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="98"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
       <c r="S6" s="9"/>
@@ -13946,23 +13946,23 @@
     </row>
     <row r="25" spans="1:45">
       <c r="A25" s="55"/>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-      <c r="O25" s="98"/>
-      <c r="P25" s="99"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="101"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -15845,8 +15845,8 @@
   </sheetPr>
   <dimension ref="A1:AO70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AU200" sqref="AU200"/>
+    <sheetView tabSelected="1" topLeftCell="F37" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -15906,7 +15906,7 @@
         <v>3.0200000000000001E-2</v>
       </c>
       <c r="I4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="13.9">
@@ -15935,10 +15935,10 @@
         <v>8.3900000000000002E-2</v>
       </c>
       <c r="H6" s="66" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I6" s="66" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" s="67"/>
       <c r="K6" s="67"/>
@@ -15967,49 +15967,49 @@
         <v>3.7199999999999997E-2</v>
       </c>
       <c r="H7" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="I7" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="K7" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="J7" s="67" t="s">
+      <c r="L7" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="K7" s="67" t="s">
+      <c r="M7" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="67" t="s">
+      <c r="N7" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="M7" s="67" t="s">
+      <c r="O7" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="67" t="s">
+      <c r="P7" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="O7" s="67" t="s">
+      <c r="Q7" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="67" t="s">
+      <c r="R7" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="Q7" s="67" t="s">
+      <c r="S7" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="R7" s="67" t="s">
+      <c r="T7" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="S7" s="67" t="s">
+      <c r="U7" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="T7" s="67" t="s">
+      <c r="V7" s="67" t="s">
         <v>59</v>
-      </c>
-      <c r="U7" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="V7" s="67" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="13.9">
@@ -16031,7 +16031,7 @@
         <v>1203998</v>
       </c>
       <c r="H8" s="68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I8" s="67">
         <v>530364</v>
@@ -16094,7 +16094,7 @@
       </c>
       <c r="E9" s="61"/>
       <c r="H9" s="68" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I9" s="67">
         <v>1266288</v>
@@ -16152,7 +16152,7 @@
         <v>0.18099999999999999</v>
       </c>
       <c r="H10" s="68" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I10" s="67">
         <v>1796652</v>
@@ -16236,7 +16236,7 @@
         <v>0.37680000000000002</v>
       </c>
       <c r="I13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="13.9">
@@ -16339,7 +16339,7 @@
         <v>0.66559999999999997</v>
       </c>
       <c r="I17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:41" ht="13.9">
@@ -16379,7 +16379,7 @@
     </row>
     <row r="21" spans="1:41">
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:41">
@@ -16549,10 +16549,10 @@
         <v>2018</v>
       </c>
       <c r="Y27" s="64" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="Z27" s="64" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="AA27" s="72">
         <v>2021</v>
@@ -16582,7 +16582,7 @@
     </row>
     <row r="28" spans="1:41">
       <c r="A28" s="64" t="s">
-        <v>43</v>
+        <v>91</v>
       </c>
       <c r="B28" s="64"/>
       <c r="C28" s="74">
@@ -16735,7 +16735,7 @@
     </row>
     <row r="30" spans="1:41">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C30" s="65">
         <v>0.129</v>
@@ -16810,7 +16810,7 @@
     </row>
     <row r="31" spans="1:41">
       <c r="A31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C31" s="65">
         <v>9.8000000000000004E-2</v>
@@ -16888,7 +16888,7 @@
     </row>
     <row r="32" spans="1:41">
       <c r="A32" t="s">
-        <v>44</v>
+        <v>90</v>
       </c>
       <c r="C32" s="65">
         <f t="shared" ref="C32" si="2">C29/C28</f>
@@ -16986,7 +16986,7 @@
     </row>
     <row r="33" spans="1:31">
       <c r="A33" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="R33" s="70">
         <v>1674000</v>
@@ -17033,7 +17033,7 @@
     </row>
     <row r="34" spans="1:31">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C34" s="73">
         <f>C31/C32</f>
@@ -17131,7 +17131,7 @@
       <c r="P61" s="91"/>
       <c r="Q61" s="81"/>
       <c r="R61" s="90"/>
-      <c r="S61" s="102">
+      <c r="S61" s="95">
         <f>S69/E69</f>
         <v>0.62070000000000003</v>
       </c>
@@ -17158,104 +17158,104 @@
     </row>
     <row r="64" spans="2:21">
       <c r="B64" t="s">
+        <v>77</v>
+      </c>
+      <c r="N64" t="s">
         <v>79</v>
       </c>
-      <c r="N64" t="s">
+      <c r="O64" t="s">
+        <v>80</v>
+      </c>
+      <c r="P64" t="s">
         <v>81</v>
       </c>
-      <c r="O64" t="s">
+      <c r="Q64" t="s">
+        <v>78</v>
+      </c>
+      <c r="R64" t="s">
         <v>82</v>
       </c>
-      <c r="P64" t="s">
+      <c r="S64" t="s">
         <v>83</v>
       </c>
-      <c r="Q64" t="s">
-        <v>80</v>
-      </c>
-      <c r="R64" t="s">
-        <v>84</v>
-      </c>
-      <c r="S64" t="s">
-        <v>85</v>
-      </c>
       <c r="T64" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="U64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="13.15">
       <c r="A66" s="76" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B66" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="C66" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="78" t="s">
+      <c r="E66" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="D66" s="78" t="s">
+      <c r="F66" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="E66" s="78" t="s">
+      <c r="G66" s="78" t="s">
         <v>51</v>
       </c>
-      <c r="F66" s="78" t="s">
+      <c r="H66" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="G66" s="78" t="s">
+      <c r="I66" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="H66" s="78" t="s">
+      <c r="J66" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="I66" s="78" t="s">
+      <c r="K66" s="78" t="s">
         <v>55</v>
       </c>
-      <c r="J66" s="78" t="s">
+      <c r="L66" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="K66" s="78" t="s">
+      <c r="M66" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="L66" s="78" t="s">
+      <c r="N66" s="78" t="s">
         <v>58</v>
       </c>
-      <c r="M66" s="78" t="s">
-        <v>59</v>
-      </c>
-      <c r="N66" s="78" t="s">
-        <v>60</v>
-      </c>
       <c r="O66" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="P66" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q66" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="P66" s="78" t="s">
+      <c r="R66" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="Q66" s="78" t="s">
+      <c r="S66" s="94">
+        <v>2019</v>
+      </c>
+      <c r="T66" s="94">
+        <v>2020</v>
+      </c>
+      <c r="U66" s="94">
+        <v>2021</v>
+      </c>
+      <c r="V66" s="78" t="s">
         <v>76</v>
-      </c>
-      <c r="R66" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="S66" s="101">
-        <v>2019</v>
-      </c>
-      <c r="T66" s="101">
-        <v>2020</v>
-      </c>
-      <c r="U66" s="101">
-        <v>2021</v>
-      </c>
-      <c r="V66" s="78" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:22">
       <c r="A67" s="68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B67" s="75">
         <v>530364</v>
@@ -17323,7 +17323,7 @@
     </row>
     <row r="68" spans="1:22">
       <c r="A68" s="68" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B68" s="75">
         <v>1266288</v>
@@ -17391,7 +17391,7 @@
     </row>
     <row r="69" spans="1:22" ht="13.15">
       <c r="A69" s="77" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B69" s="79">
         <v>1796652</v>
@@ -17459,7 +17459,7 @@
     </row>
     <row r="70" spans="1:22">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B70" s="80">
         <f>B67/B68</f>
@@ -17579,12 +17579,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="15.75">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
     </row>
     <row r="2" spans="1:32">
       <c r="A2" s="2" t="s">
@@ -17696,23 +17696,23 @@
     </row>
     <row r="6" spans="1:32">
       <c r="A6" s="55"/>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="98"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="32"/>
       <c r="S6" s="14"/>
@@ -19355,23 +19355,23 @@
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="55"/>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-      <c r="O25" s="98"/>
-      <c r="P25" s="99"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="101"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
@@ -21050,12 +21050,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="15.75">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="100"/>
-      <c r="C1" s="100"/>
-      <c r="D1" s="100"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
     </row>
     <row r="2" spans="1:33">
       <c r="A2" s="2" t="s">
@@ -21168,23 +21168,23 @@
     </row>
     <row r="6" spans="1:33">
       <c r="A6" s="55"/>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="96" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
-      <c r="G6" s="95"/>
-      <c r="H6" s="95"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="95"/>
-      <c r="O6" s="95"/>
-      <c r="P6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="97"/>
+      <c r="E6" s="97"/>
+      <c r="F6" s="97"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="97"/>
+      <c r="I6" s="97"/>
+      <c r="J6" s="97"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="97"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="97"/>
+      <c r="O6" s="97"/>
+      <c r="P6" s="98"/>
       <c r="Q6" s="28"/>
       <c r="R6" s="28"/>
       <c r="S6" s="28"/>
@@ -22845,23 +22845,23 @@
     </row>
     <row r="25" spans="1:33">
       <c r="A25" s="55"/>
-      <c r="B25" s="97" t="s">
+      <c r="B25" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="98"/>
-      <c r="D25" s="98"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="98"/>
-      <c r="G25" s="98"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="98"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="98"/>
-      <c r="M25" s="98"/>
-      <c r="N25" s="98"/>
-      <c r="O25" s="98"/>
-      <c r="P25" s="99"/>
+      <c r="C25" s="100"/>
+      <c r="D25" s="100"/>
+      <c r="E25" s="100"/>
+      <c r="F25" s="100"/>
+      <c r="G25" s="100"/>
+      <c r="H25" s="100"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="100"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="100"/>
+      <c r="M25" s="100"/>
+      <c r="N25" s="100"/>
+      <c r="O25" s="100"/>
+      <c r="P25" s="101"/>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -24552,26 +24552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TemplateUrl xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <NazwaPliku xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373">tablica_1.xls.xls</NazwaPliku>
-    <_SourceUrl xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Odbiorcy2 xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373" xsi:nil="true"/>
-    <xd_ProgID xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Osoba xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373">STAT\FRANECKAA</Osoba>
-    <Order xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_SharedFileIndex xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <MetaInfo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Pisma" ma:contentTypeID="0x003F9B028CC42C594AAF0DA90575FA3373" ma:contentTypeVersion="" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="a80ed856fbc5a997d44bfc997ced819f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="8C029B3F-2CC4-4A59-AF0D-A90575FA3373" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e61943d334749cc2f7f8fac3c3188088" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25060,10 +25040,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TemplateUrl xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <NazwaPliku xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373">tablica_1.xls.xls</NazwaPliku>
+    <_SourceUrl xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Odbiorcy2 xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373" xsi:nil="true"/>
+    <xd_ProgID xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Osoba xmlns="8C029B3F-2CC4-4A59-AF0D-A90575FA3373">STAT\FRANECKAA</Osoba>
+    <Order xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_SharedFileIndex xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <MetaInfo xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{103376CD-359E-47F9-AEA5-A14028D9900D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD695C88-BE97-4863-A283-EFBBD960D164}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="8C029B3F-2CC4-4A59-AF0D-A90575FA3373"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -25080,20 +25091,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD695C88-BE97-4863-A283-EFBBD960D164}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{103376CD-359E-47F9-AEA5-A14028D9900D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="8C029B3F-2CC4-4A59-AF0D-A90575FA3373"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>